<commit_message>
updates: rm id in expense and funding for user
</commit_message>
<xml_diff>
--- a/test/base_test.xlsx
+++ b/test/base_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/limnaroline/forecasting-project/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Intern\WEHI\prod\forecasting-with-workday-project\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2108A0F-D16C-1749-8CF8-C49E2E348552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C12C36-284A-423E-8C92-30B9D6FA4CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20080" yWindow="2860" windowWidth="14000" windowHeight="14360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2508" yWindow="2508" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funding" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
-  <si>
-    <t>Source ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Funding Source</t>
   </si>
@@ -47,9 +44,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>Expense ID</t>
-  </si>
-  <si>
     <t>Expense Name</t>
   </si>
   <si>
@@ -62,27 +56,6 @@
     <t>Latest Payment Date</t>
   </si>
   <si>
-    <t>F001</t>
-  </si>
-  <si>
-    <t>F002</t>
-  </si>
-  <si>
-    <t>F003</t>
-  </si>
-  <si>
-    <t>F004</t>
-  </si>
-  <si>
-    <t>F005</t>
-  </si>
-  <si>
-    <t>F006</t>
-  </si>
-  <si>
-    <t>F007</t>
-  </si>
-  <si>
     <t>Salary</t>
   </si>
   <si>
@@ -111,36 +84,6 @@
   </si>
   <si>
     <t>Funding G</t>
-  </si>
-  <si>
-    <t>E001</t>
-  </si>
-  <si>
-    <t>E002</t>
-  </si>
-  <si>
-    <t>E003</t>
-  </si>
-  <si>
-    <t>E004</t>
-  </si>
-  <si>
-    <t>E005</t>
-  </si>
-  <si>
-    <t>E006</t>
-  </si>
-  <si>
-    <t>E007</t>
-  </si>
-  <si>
-    <t>E008</t>
-  </si>
-  <si>
-    <t>E009</t>
-  </si>
-  <si>
-    <t>E010</t>
   </si>
   <si>
     <t>Tom's salary</t>
@@ -511,19 +454,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,147 +485,123 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45658</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45747</v>
+      </c>
+      <c r="E2">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45689</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45838</v>
+      </c>
+      <c r="E3">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C4" s="1">
+        <v>45748</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45930</v>
+      </c>
+      <c r="E4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45658</v>
+      </c>
+      <c r="D5" s="1">
+        <v>46022</v>
+      </c>
+      <c r="E5">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D6" s="1">
+        <v>46022</v>
+      </c>
+      <c r="E6">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45658</v>
+      </c>
+      <c r="D7" s="1">
+        <v>46022</v>
+      </c>
+      <c r="E7">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1">
-        <v>45658</v>
-      </c>
-      <c r="E2" s="1">
-        <v>45747</v>
-      </c>
-      <c r="F2">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1">
-        <v>45689</v>
-      </c>
-      <c r="E3" s="1">
-        <v>45838</v>
-      </c>
-      <c r="F3">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="1">
-        <v>45748</v>
-      </c>
-      <c r="E4" s="1">
-        <v>45930</v>
-      </c>
-      <c r="F4">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1">
-        <v>45658</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D8" s="1">
         <v>46022</v>
       </c>
-      <c r="F5">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1">
-        <v>45839</v>
-      </c>
-      <c r="E6" s="1">
-        <v>46022</v>
-      </c>
-      <c r="F6">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1">
-        <v>45658</v>
-      </c>
-      <c r="E7" s="1">
-        <v>46022</v>
-      </c>
-      <c r="F7">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="1">
-        <v>45931</v>
-      </c>
-      <c r="E8" s="1">
-        <v>46022</v>
-      </c>
-      <c r="F8">
+      <c r="E8">
         <v>9000</v>
       </c>
     </row>
@@ -695,244 +614,211 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="160" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" customWidth="1"/>
-    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
       <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2">
+        <v>11</v>
+      </c>
+      <c r="D2">
         <v>9000</v>
       </c>
-      <c r="F2" s="1">
+      <c r="E2" s="1">
         <v>45672</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="D3">
         <v>40000</v>
       </c>
-      <c r="F3" s="1">
+      <c r="E3" s="1">
         <v>45708</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4">
+        <v>11</v>
+      </c>
+      <c r="D4">
         <v>8000</v>
       </c>
-      <c r="F4" s="1">
+      <c r="E4" s="1">
         <v>45726</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5">
+        <v>13</v>
+      </c>
+      <c r="D5">
         <v>6000</v>
       </c>
-      <c r="F5" s="1">
+      <c r="E5" s="1">
         <v>45752</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="D6">
         <v>15000</v>
       </c>
-      <c r="F6" s="1">
+      <c r="E6" s="1">
         <v>45792</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7">
+        <v>11</v>
+      </c>
+      <c r="D7">
         <v>20000</v>
       </c>
-      <c r="F7" s="1">
+      <c r="E7" s="1">
         <v>45818</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8">
+        <v>13</v>
+      </c>
+      <c r="D8">
         <v>7000</v>
       </c>
-      <c r="F8" s="1">
+      <c r="E8" s="1">
         <v>45858</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9">
+        <v>12</v>
+      </c>
+      <c r="D9">
         <v>9000</v>
       </c>
-      <c r="F9" s="1">
+      <c r="E9" s="1">
         <v>45899</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10">
+        <v>11</v>
+      </c>
+      <c r="D10">
         <v>12000</v>
       </c>
-      <c r="F10" s="1">
+      <c r="E10" s="1">
         <v>45931</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11">
+        <v>13</v>
+      </c>
+      <c r="D11">
         <v>5000</v>
       </c>
-      <c r="F11" s="1">
+      <c r="E11" s="1">
         <v>45976</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F12" s="1"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>